<commit_message>
archivos generafos por tune_config
</commit_message>
<xml_diff>
--- a/outputs/backtest_plots/EURUSD_backtest_consolidado.xlsx
+++ b/outputs/backtest_plots/EURUSD_backtest_consolidado.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="145">
   <si>
     <t>model</t>
   </si>
@@ -125,6 +125,9 @@
     <t>param.enforce_invertibility</t>
   </si>
   <si>
+    <t>param.order</t>
+  </si>
+  <si>
     <t>EURUSD</t>
   </si>
   <si>
@@ -134,15 +137,12 @@
     <t>fixed</t>
   </si>
   <si>
-    <t>True</t>
+    <t>False</t>
   </si>
   <si>
     <t>aic</t>
   </si>
   <si>
-    <t>False</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -155,6 +155,9 @@
     <t>1</t>
   </si>
   <si>
+    <t>[0, 1, 2]</t>
+  </si>
+  <si>
     <t>y_pred</t>
   </si>
   <si>
@@ -203,10 +206,10 @@
     <t>D1</t>
   </si>
   <si>
-    <t>0.05</t>
-  </si>
-  <si>
-    <t>additive</t>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>multiplicative</t>
   </si>
   <si>
     <t>param.window</t>
@@ -323,6 +326,12 @@
     <t>modelo.params.enforce_invertibility</t>
   </si>
   <si>
+    <t>validacion.modo</t>
+  </si>
+  <si>
+    <t>validacion.n</t>
+  </si>
+  <si>
     <t>modelos</t>
   </si>
   <si>
@@ -401,13 +410,16 @@
     <t>D</t>
   </si>
   <si>
-    <t>[1, 1, 1]</t>
-  </si>
-  <si>
     <t>[0, 0, 0, 0]</t>
   </si>
   <si>
-    <t>[{'name': 'ARIMA', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'auto': True, 'metric': 'aic', 'seasonal': False, 'm': 12, 'modo': 'retornos', 'max_p': 2, 'max_q': 2, 'max_P': 2, 'max_Q': 2, 'max_d': 2, 'max_D': 1, 'enforce_stationarity': False, 'enforce_invertibility': False}, 'normal': {}, 'backtest': {'engine': 'model'}}, {'name': 'RW', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'order': [0, 1, 0], 'seasonal_order': [0, 0, 0, 0], 'enforce_stationarity': False, 'enforce_invertibility': False}, 'normal': {}, 'backtest': {'engine': 'classic_auto'}}, {'name': 'PROPHET', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'frequency_hint': 'D1', 'changepoint_prior_scale': 0.05, 'seasonality_mode': 'additive'}, 'normal': {}, 'backtest': {'engine': 'model', 'prophet': {'frequency_hint': 'D1', 'yearly_seasonality': False, 'weekly_seasonality': True, 'daily_seasonality': True, 'interval_width': 0.9}}}, {'name': 'LSTM', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'window': 64, 'units': 64, 'dropout': 0.2, 'epochs': 40, 'batch_size': 32, 'lr': 0.001, 'loss': 'mse', 'optimizer': 'adam', 'scaler': 'standard', 'patience': 5, 'model_dir': 'outputs/modelos/lstm'}, 'normal': {}, 'backtest': {'engine': 'model', 'lstm': {'horizon': 5}}}]</t>
+    <t>last_n</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>[{'name': 'ARIMA', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'auto': False, 'metric': 'aic', 'seasonal': False, 'm': 12, 'modo': 'retornos', 'max_p': 2, 'max_q': 2, 'max_P': 2, 'max_Q': 2, 'max_d': 2, 'max_D': 1, 'enforce_stationarity': False, 'enforce_invertibility': False, 'order': [0, 1, 2]}, 'normal': {}, 'backtest': {'engine': 'model'}}, {'name': 'RW', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'order': [0, 1, 0], 'seasonal_order': [0, 0, 0, 0], 'enforce_stationarity': False, 'enforce_invertibility': False}, 'normal': {}, 'backtest': {'engine': 'classic_auto'}}, {'name': 'PROPHET', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'frequency_hint': 'D1', 'changepoint_prior_scale': 0.5, 'seasonality_mode': 'multiplicative'}, 'normal': {}, 'backtest': {'engine': 'model', 'prophet': {'frequency_hint': 'D1', 'yearly_seasonality': False, 'weekly_seasonality': True, 'daily_seasonality': True, 'interval_width': 0.9}}}, {'name': 'LSTM', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'window': 64, 'units': 64, 'dropout': 0.2, 'epochs': 40, 'batch_size': 32, 'lr': 0.001, 'loss': 'mse', 'optimizer': 'adam', 'scaler': 'standard', 'patience': 5, 'model_dir': 'outputs/modelos/lstm'}, 'normal': {}, 'backtest': {'engine': 'model', 'lstm': {'horizon': 5}}}]</t>
   </si>
   <si>
     <t>800</t>
@@ -894,13 +906,13 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.007124026660919206</v>
+        <v>0.007087012176513688</v>
       </c>
       <c r="C4">
-        <v>0.008193976626200326</v>
+        <v>0.008231930430021343</v>
       </c>
       <c r="D4">
-        <v>0.006469863426529997</v>
+        <v>0.006454434479344</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -922,7 +934,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -941,7 +953,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -957,7 +969,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -983,7 +995,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1007,7 +1019,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1015,7 +1027,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1023,7 +1035,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1095,7 +1107,7 @@
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -1103,157 +1115,106 @@
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="1">
-        <v>1</v>
-      </c>
-      <c r="B25" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <v>3</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>4</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E26" s="1">
         <v>5</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="L26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P25" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="Q26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="S26" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19">
-      <c r="A26">
-        <v>1.06089</v>
-      </c>
-      <c r="B26">
-        <v>1.06089</v>
-      </c>
-      <c r="C26">
-        <v>1.06089</v>
-      </c>
-      <c r="D26">
-        <v>1.06089</v>
-      </c>
-      <c r="E26">
-        <v>1.06089</v>
-      </c>
-      <c r="F26">
-        <v>1.06089</v>
-      </c>
-      <c r="G26">
-        <v>1.05737</v>
-      </c>
-      <c r="H26">
-        <v>-0.00352000000000019</v>
-      </c>
-      <c r="I26">
-        <v>0.00352000000000019</v>
-      </c>
-      <c r="J26">
-        <v>1.239040000000134E-05</v>
-      </c>
-      <c r="M26">
-        <v>1</v>
-      </c>
-      <c r="N26">
-        <v>12</v>
-      </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
-        <v>1.05737</v>
-      </c>
-      <c r="Q26">
-        <v>1.05737</v>
-      </c>
-      <c r="R26" s="2">
-        <v>43864</v>
-      </c>
-      <c r="S26" s="2">
-        <v>44985</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27">
-        <v>1.10035</v>
+        <v>1.06089</v>
       </c>
       <c r="B27">
-        <v>1.10035</v>
+        <v>1.06089</v>
       </c>
       <c r="C27">
-        <v>1.10035</v>
+        <v>1.06089</v>
       </c>
       <c r="D27">
-        <v>1.10035</v>
+        <v>1.06089</v>
       </c>
       <c r="E27">
-        <v>1.10035</v>
+        <v>1.06089</v>
       </c>
       <c r="F27">
-        <v>1.10035</v>
+        <v>1.06089</v>
       </c>
       <c r="G27">
-        <v>1.09597</v>
+        <v>1.05737</v>
       </c>
       <c r="H27">
-        <v>-0.004380000000000051</v>
+        <v>-0.00352000000000019</v>
       </c>
       <c r="I27">
-        <v>0.004380000000000051</v>
+        <v>0.00352000000000019</v>
       </c>
       <c r="J27">
-        <v>1.918440000000044E-05</v>
-      </c>
-      <c r="K27" t="s">
-        <v>55</v>
-      </c>
-      <c r="L27" t="s">
-        <v>55</v>
+        <v>1.239040000000134E-05</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -1265,54 +1226,54 @@
         <v>1</v>
       </c>
       <c r="P27">
-        <v>1.09597</v>
+        <v>1.05737</v>
       </c>
       <c r="Q27">
-        <v>2.15334</v>
+        <v>1.05737</v>
       </c>
       <c r="R27" s="2">
-        <v>43934</v>
+        <v>43864</v>
       </c>
       <c r="S27" s="2">
-        <v>45055</v>
+        <v>44985</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28">
-        <v>1.12398</v>
+        <v>1.10035</v>
       </c>
       <c r="B28">
-        <v>1.12398</v>
+        <v>1.10035</v>
       </c>
       <c r="C28">
-        <v>1.12398</v>
+        <v>1.10035</v>
       </c>
       <c r="D28">
-        <v>1.12398</v>
+        <v>1.10035</v>
       </c>
       <c r="E28">
-        <v>1.12398</v>
+        <v>1.10035</v>
       </c>
       <c r="F28">
-        <v>1.12398</v>
+        <v>1.10035</v>
       </c>
       <c r="G28">
-        <v>1.12275</v>
+        <v>1.09597</v>
       </c>
       <c r="H28">
-        <v>-0.001230000000000064</v>
+        <v>-0.004380000000000051</v>
       </c>
       <c r="I28">
-        <v>0.001230000000000064</v>
+        <v>0.004380000000000051</v>
       </c>
       <c r="J28">
-        <v>1.512900000000158E-06</v>
+        <v>1.918440000000044E-05</v>
       </c>
       <c r="K28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M28">
         <v>1</v>
@@ -1324,48 +1285,48 @@
         <v>1</v>
       </c>
       <c r="P28">
-        <v>1.12275</v>
+        <v>1.09597</v>
       </c>
       <c r="Q28">
-        <v>3.27609</v>
+        <v>2.15334</v>
       </c>
       <c r="R28" s="2">
-        <v>44004</v>
+        <v>43934</v>
       </c>
       <c r="S28" s="2">
-        <v>45125</v>
+        <v>45055</v>
       </c>
     </row>
     <row r="29" spans="1:19">
       <c r="A29">
-        <v>1.05919</v>
+        <v>1.12398</v>
       </c>
       <c r="B29">
-        <v>1.05919</v>
+        <v>1.12398</v>
       </c>
       <c r="C29">
-        <v>1.05919</v>
+        <v>1.12398</v>
       </c>
       <c r="D29">
-        <v>1.05919</v>
+        <v>1.12398</v>
       </c>
       <c r="E29">
-        <v>1.05919</v>
+        <v>1.12398</v>
       </c>
       <c r="F29">
-        <v>1.05919</v>
+        <v>1.12398</v>
       </c>
       <c r="G29">
-        <v>1.05706</v>
+        <v>1.12275</v>
       </c>
       <c r="H29">
-        <v>-0.002130000000000187</v>
+        <v>-0.001230000000000064</v>
       </c>
       <c r="I29">
-        <v>0.002130000000000187</v>
+        <v>0.001230000000000064</v>
       </c>
       <c r="J29">
-        <v>4.536900000000798E-06</v>
+        <v>1.512900000000158E-06</v>
       </c>
       <c r="K29" t="s">
         <v>56</v>
@@ -1383,54 +1344,54 @@
         <v>1</v>
       </c>
       <c r="P29">
-        <v>1.05706</v>
+        <v>1.12275</v>
       </c>
       <c r="Q29">
-        <v>4.33315</v>
+        <v>3.27609</v>
       </c>
       <c r="R29" s="2">
-        <v>44074</v>
+        <v>44004</v>
       </c>
       <c r="S29" s="2">
-        <v>45195</v>
+        <v>45125</v>
       </c>
     </row>
     <row r="30" spans="1:19">
       <c r="A30">
-        <v>1.08351</v>
+        <v>1.05919</v>
       </c>
       <c r="B30">
-        <v>1.08351</v>
+        <v>1.05919</v>
       </c>
       <c r="C30">
-        <v>1.08351</v>
+        <v>1.05919</v>
       </c>
       <c r="D30">
-        <v>1.08351</v>
+        <v>1.05919</v>
       </c>
       <c r="E30">
-        <v>1.08351</v>
+        <v>1.05919</v>
       </c>
       <c r="F30">
-        <v>1.08351</v>
+        <v>1.05919</v>
       </c>
       <c r="G30">
-        <v>1.07974</v>
+        <v>1.05706</v>
       </c>
       <c r="H30">
-        <v>-0.003770000000000051</v>
+        <v>-0.002130000000000187</v>
       </c>
       <c r="I30">
-        <v>0.003770000000000051</v>
+        <v>0.002130000000000187</v>
       </c>
       <c r="J30">
-        <v>1.421290000000039E-05</v>
+        <v>4.536900000000798E-06</v>
       </c>
       <c r="K30" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L30" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -1442,48 +1403,48 @@
         <v>1</v>
       </c>
       <c r="P30">
-        <v>1.07974</v>
+        <v>1.05706</v>
       </c>
       <c r="Q30">
-        <v>5.41289</v>
+        <v>4.33315</v>
       </c>
       <c r="R30" s="2">
-        <v>44144</v>
+        <v>44074</v>
       </c>
       <c r="S30" s="2">
-        <v>45265</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="A31">
-        <v>1.07274</v>
+        <v>1.08351</v>
       </c>
       <c r="B31">
-        <v>1.07274</v>
+        <v>1.08351</v>
       </c>
       <c r="C31">
-        <v>1.07274</v>
+        <v>1.08351</v>
       </c>
       <c r="D31">
-        <v>1.07274</v>
+        <v>1.08351</v>
       </c>
       <c r="E31">
-        <v>1.07274</v>
+        <v>1.08351</v>
       </c>
       <c r="F31">
-        <v>1.07274</v>
+        <v>1.08351</v>
       </c>
       <c r="G31">
-        <v>1.07728</v>
+        <v>1.07974</v>
       </c>
       <c r="H31">
-        <v>0.004539999999999988</v>
+        <v>-0.003770000000000051</v>
       </c>
       <c r="I31">
-        <v>0.004539999999999988</v>
+        <v>0.003770000000000051</v>
       </c>
       <c r="J31">
-        <v>2.06115999999999E-05</v>
+        <v>1.421290000000039E-05</v>
       </c>
       <c r="K31" t="s">
         <v>56</v>
@@ -1501,54 +1462,54 @@
         <v>1</v>
       </c>
       <c r="P31">
-        <v>1.07728</v>
+        <v>1.07974</v>
       </c>
       <c r="Q31">
-        <v>6.49017</v>
+        <v>5.41289</v>
       </c>
       <c r="R31" s="2">
-        <v>44216</v>
+        <v>44144</v>
       </c>
       <c r="S31" s="2">
-        <v>45337</v>
+        <v>45265</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32">
-        <v>1.06982</v>
+        <v>1.07274</v>
       </c>
       <c r="B32">
-        <v>1.06982</v>
+        <v>1.07274</v>
       </c>
       <c r="C32">
-        <v>1.06982</v>
+        <v>1.07274</v>
       </c>
       <c r="D32">
-        <v>1.06982</v>
+        <v>1.07274</v>
       </c>
       <c r="E32">
-        <v>1.06982</v>
+        <v>1.07274</v>
       </c>
       <c r="F32">
-        <v>1.06982</v>
+        <v>1.07274</v>
       </c>
       <c r="G32">
-        <v>1.07297</v>
+        <v>1.07728</v>
       </c>
       <c r="H32">
-        <v>0.003149999999999986</v>
+        <v>0.004539999999999988</v>
       </c>
       <c r="I32">
-        <v>0.003149999999999986</v>
+        <v>0.004539999999999988</v>
       </c>
       <c r="J32">
-        <v>9.922499999999912E-06</v>
+        <v>2.06115999999999E-05</v>
       </c>
       <c r="K32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -1560,54 +1521,54 @@
         <v>1</v>
       </c>
       <c r="P32">
-        <v>1.07297</v>
+        <v>1.07728</v>
       </c>
       <c r="Q32">
-        <v>7.56314</v>
+        <v>6.49017</v>
       </c>
       <c r="R32" s="2">
-        <v>44286</v>
+        <v>44216</v>
       </c>
       <c r="S32" s="2">
-        <v>45407</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="33" spans="1:19">
       <c r="A33">
-        <v>1.0788</v>
+        <v>1.06982</v>
       </c>
       <c r="B33">
-        <v>1.0788</v>
+        <v>1.06982</v>
       </c>
       <c r="C33">
-        <v>1.0788</v>
+        <v>1.06982</v>
       </c>
       <c r="D33">
-        <v>1.0788</v>
+        <v>1.06982</v>
       </c>
       <c r="E33">
-        <v>1.0788</v>
+        <v>1.06982</v>
       </c>
       <c r="F33">
-        <v>1.0788</v>
+        <v>1.06982</v>
       </c>
       <c r="G33">
-        <v>1.0811</v>
+        <v>1.07297</v>
       </c>
       <c r="H33">
-        <v>0.002299999999999969</v>
+        <v>0.003149999999999986</v>
       </c>
       <c r="I33">
-        <v>0.002299999999999969</v>
+        <v>0.003149999999999986</v>
       </c>
       <c r="J33">
-        <v>5.289999999999856E-06</v>
+        <v>9.922499999999912E-06</v>
       </c>
       <c r="K33" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L33" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M33">
         <v>1</v>
@@ -1619,54 +1580,54 @@
         <v>1</v>
       </c>
       <c r="P33">
-        <v>1.0811</v>
+        <v>1.07297</v>
       </c>
       <c r="Q33">
-        <v>8.64424</v>
+        <v>7.56314</v>
       </c>
       <c r="R33" s="2">
-        <v>44356</v>
+        <v>44286</v>
       </c>
       <c r="S33" s="2">
-        <v>45477</v>
+        <v>45407</v>
       </c>
     </row>
     <row r="34" spans="1:19">
       <c r="A34">
-        <v>1.10136</v>
+        <v>1.0788</v>
       </c>
       <c r="B34">
-        <v>1.10136</v>
+        <v>1.0788</v>
       </c>
       <c r="C34">
-        <v>1.10136</v>
+        <v>1.0788</v>
       </c>
       <c r="D34">
-        <v>1.10136</v>
+        <v>1.0788</v>
       </c>
       <c r="E34">
-        <v>1.10136</v>
+        <v>1.0788</v>
       </c>
       <c r="F34">
-        <v>1.10136</v>
+        <v>1.0788</v>
       </c>
       <c r="G34">
-        <v>1.10726</v>
+        <v>1.0811</v>
       </c>
       <c r="H34">
-        <v>0.005899999999999794</v>
+        <v>0.002299999999999969</v>
       </c>
       <c r="I34">
-        <v>0.005899999999999794</v>
+        <v>0.002299999999999969</v>
       </c>
       <c r="J34">
-        <v>3.480999999999757E-05</v>
+        <v>5.289999999999856E-06</v>
       </c>
       <c r="K34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M34">
         <v>1</v>
@@ -1678,48 +1639,48 @@
         <v>1</v>
       </c>
       <c r="P34">
-        <v>1.10726</v>
+        <v>1.0811</v>
       </c>
       <c r="Q34">
-        <v>9.7515</v>
+        <v>8.64424</v>
       </c>
       <c r="R34" s="2">
-        <v>44426</v>
+        <v>44356</v>
       </c>
       <c r="S34" s="2">
-        <v>45547</v>
+        <v>45477</v>
       </c>
     </row>
     <row r="35" spans="1:19">
       <c r="A35">
-        <v>1.05428</v>
+        <v>1.10136</v>
       </c>
       <c r="B35">
-        <v>1.05428</v>
+        <v>1.10136</v>
       </c>
       <c r="C35">
-        <v>1.05428</v>
+        <v>1.10136</v>
       </c>
       <c r="D35">
-        <v>1.05428</v>
+        <v>1.10136</v>
       </c>
       <c r="E35">
-        <v>1.05428</v>
+        <v>1.10136</v>
       </c>
       <c r="F35">
-        <v>1.05428</v>
+        <v>1.10136</v>
       </c>
       <c r="G35">
-        <v>1.0472</v>
+        <v>1.10726</v>
       </c>
       <c r="H35">
-        <v>-0.007080000000000197</v>
+        <v>0.005899999999999794</v>
       </c>
       <c r="I35">
-        <v>0.007080000000000197</v>
+        <v>0.005899999999999794</v>
       </c>
       <c r="J35">
-        <v>5.012640000000279E-05</v>
+        <v>3.480999999999757E-05</v>
       </c>
       <c r="K35" t="s">
         <v>56</v>
@@ -1737,54 +1698,54 @@
         <v>1</v>
       </c>
       <c r="P35">
-        <v>1.0472</v>
+        <v>1.10726</v>
       </c>
       <c r="Q35">
-        <v>10.7987</v>
+        <v>9.7515</v>
       </c>
       <c r="R35" s="2">
-        <v>44496</v>
+        <v>44426</v>
       </c>
       <c r="S35" s="2">
-        <v>45617</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="36" spans="1:19">
       <c r="A36">
-        <v>1.03575</v>
+        <v>1.05428</v>
       </c>
       <c r="B36">
-        <v>1.03575</v>
+        <v>1.05428</v>
       </c>
       <c r="C36">
-        <v>1.03575</v>
+        <v>1.05428</v>
       </c>
       <c r="D36">
-        <v>1.03575</v>
+        <v>1.05428</v>
       </c>
       <c r="E36">
-        <v>1.03575</v>
+        <v>1.05428</v>
       </c>
       <c r="F36">
-        <v>1.03575</v>
+        <v>1.05428</v>
       </c>
       <c r="G36">
-        <v>1.03342</v>
+        <v>1.0472</v>
       </c>
       <c r="H36">
-        <v>-0.002329999999999943</v>
+        <v>-0.007080000000000197</v>
       </c>
       <c r="I36">
-        <v>0.002329999999999943</v>
+        <v>0.007080000000000197</v>
       </c>
       <c r="J36">
-        <v>5.428899999999736E-06</v>
+        <v>5.012640000000279E-05</v>
       </c>
       <c r="K36" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L36" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M36">
         <v>1</v>
@@ -1796,54 +1757,54 @@
         <v>1</v>
       </c>
       <c r="P36">
-        <v>1.03342</v>
+        <v>1.0472</v>
       </c>
       <c r="Q36">
-        <v>11.83212</v>
+        <v>10.7987</v>
       </c>
       <c r="R36" s="2">
-        <v>44566</v>
+        <v>44496</v>
       </c>
       <c r="S36" s="2">
-        <v>45691</v>
+        <v>45617</v>
       </c>
     </row>
     <row r="37" spans="1:19">
       <c r="A37">
-        <v>1.13509</v>
+        <v>1.03575</v>
       </c>
       <c r="B37">
-        <v>1.13509</v>
+        <v>1.03575</v>
       </c>
       <c r="C37">
-        <v>1.13509</v>
+        <v>1.03575</v>
       </c>
       <c r="D37">
-        <v>1.13509</v>
+        <v>1.03575</v>
       </c>
       <c r="E37">
-        <v>1.13509</v>
+        <v>1.03575</v>
       </c>
       <c r="F37">
-        <v>1.13509</v>
+        <v>1.03575</v>
       </c>
       <c r="G37">
-        <v>1.13503</v>
+        <v>1.03342</v>
       </c>
       <c r="H37">
-        <v>-5.999999999994898E-05</v>
+        <v>-0.002329999999999943</v>
       </c>
       <c r="I37">
-        <v>5.999999999994898E-05</v>
+        <v>0.002329999999999943</v>
       </c>
       <c r="J37">
-        <v>3.599999999993878E-09</v>
+        <v>5.428899999999736E-06</v>
       </c>
       <c r="K37" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L37" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M37">
         <v>1</v>
@@ -1855,54 +1816,54 @@
         <v>1</v>
       </c>
       <c r="P37">
-        <v>1.13503</v>
+        <v>1.03342</v>
       </c>
       <c r="Q37">
-        <v>12.96715</v>
+        <v>11.83212</v>
       </c>
       <c r="R37" s="2">
-        <v>44636</v>
+        <v>44566</v>
       </c>
       <c r="S37" s="2">
-        <v>45761</v>
+        <v>45691</v>
       </c>
     </row>
     <row r="38" spans="1:19">
       <c r="A38">
-        <v>1.15216</v>
+        <v>1.13509</v>
       </c>
       <c r="B38">
-        <v>1.15216</v>
+        <v>1.13509</v>
       </c>
       <c r="C38">
-        <v>1.15216</v>
+        <v>1.13509</v>
       </c>
       <c r="D38">
-        <v>1.15216</v>
+        <v>1.13509</v>
       </c>
       <c r="E38">
-        <v>1.15216</v>
+        <v>1.13509</v>
       </c>
       <c r="F38">
-        <v>1.15216</v>
+        <v>1.13509</v>
       </c>
       <c r="G38">
-        <v>1.15777</v>
+        <v>1.13503</v>
       </c>
       <c r="H38">
-        <v>0.005609999999999893</v>
+        <v>-5.999999999994898E-05</v>
       </c>
       <c r="I38">
-        <v>0.005609999999999893</v>
+        <v>5.999999999994898E-05</v>
       </c>
       <c r="J38">
-        <v>3.14720999999988E-05</v>
+        <v>3.599999999993878E-09</v>
       </c>
       <c r="K38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M38">
         <v>1</v>
@@ -1914,74 +1875,133 @@
         <v>1</v>
       </c>
       <c r="P38">
-        <v>1.15777</v>
+        <v>1.13503</v>
       </c>
       <c r="Q38">
-        <v>14.12492</v>
+        <v>12.96715</v>
       </c>
       <c r="R38" s="2">
-        <v>44706</v>
+        <v>44636</v>
       </c>
       <c r="S38" s="2">
-        <v>45831</v>
+        <v>45761</v>
       </c>
     </row>
     <row r="39" spans="1:19">
       <c r="A39">
+        <v>1.15216</v>
+      </c>
+      <c r="B39">
+        <v>1.15216</v>
+      </c>
+      <c r="C39">
+        <v>1.15216</v>
+      </c>
+      <c r="D39">
+        <v>1.15216</v>
+      </c>
+      <c r="E39">
+        <v>1.15216</v>
+      </c>
+      <c r="F39">
+        <v>1.15216</v>
+      </c>
+      <c r="G39">
+        <v>1.15777</v>
+      </c>
+      <c r="H39">
+        <v>0.005609999999999893</v>
+      </c>
+      <c r="I39">
+        <v>0.005609999999999893</v>
+      </c>
+      <c r="J39">
+        <v>3.14720999999988E-05</v>
+      </c>
+      <c r="K39" t="s">
+        <v>56</v>
+      </c>
+      <c r="L39" t="s">
+        <v>56</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>12</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <v>1.15777</v>
+      </c>
+      <c r="Q39">
+        <v>14.12492</v>
+      </c>
+      <c r="R39" s="2">
+        <v>44706</v>
+      </c>
+      <c r="S39" s="2">
+        <v>45831</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="A40">
         <v>1.16863</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>1.16863</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>1.16863</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>1.16863</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>1.16863</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <v>1.16863</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>1.17117</v>
       </c>
-      <c r="H39">
+      <c r="H40">
         <v>0.002539999999999987</v>
       </c>
-      <c r="I39">
+      <c r="I40">
         <v>0.002539999999999987</v>
       </c>
-      <c r="J39">
+      <c r="J40">
         <v>6.451599999999932E-06</v>
       </c>
-      <c r="K39" t="s">
-        <v>55</v>
-      </c>
-      <c r="L39" t="s">
-        <v>55</v>
-      </c>
-      <c r="M39">
-        <v>1</v>
-      </c>
-      <c r="N39">
-        <v>12</v>
-      </c>
-      <c r="O39">
-        <v>1</v>
-      </c>
-      <c r="P39">
+      <c r="K40" t="s">
+        <v>56</v>
+      </c>
+      <c r="L40" t="s">
+        <v>56</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>12</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
         <v>1.17117</v>
       </c>
-      <c r="Q39">
+      <c r="Q40">
         <v>15.29609</v>
       </c>
-      <c r="R39" s="2">
+      <c r="R40" s="2">
         <v>44776</v>
       </c>
-      <c r="S39" s="2">
+      <c r="S40" s="2">
         <v>45901</v>
       </c>
     </row>
@@ -2011,7 +2031,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2027,7 +2047,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2053,7 +2073,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -2074,26 +2094,26 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -2113,25 +2133,25 @@
         <v>5</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>16</v>
@@ -2140,13 +2160,13 @@
         <v>20</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>7</v>
@@ -2240,10 +2260,10 @@
         <v>6.88292986816285E-05</v>
       </c>
       <c r="K17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -2299,10 +2319,10 @@
         <v>0.0007357762934999373</v>
       </c>
       <c r="K18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -2358,10 +2378,10 @@
         <v>0.0001358927601151433</v>
       </c>
       <c r="K19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -2417,10 +2437,10 @@
         <v>0.0004298098324425534</v>
       </c>
       <c r="K20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -2476,10 +2496,10 @@
         <v>6.133196370391123E-06</v>
       </c>
       <c r="K21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -2535,10 +2555,10 @@
         <v>7.231732186668922E-06</v>
       </c>
       <c r="K22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -2594,10 +2614,10 @@
         <v>0.0001206596967869473</v>
       </c>
       <c r="K23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -2653,10 +2673,10 @@
         <v>3.367328350517297E-06</v>
       </c>
       <c r="K24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -2712,10 +2732,10 @@
         <v>0.001375835335882608</v>
       </c>
       <c r="K25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -2771,10 +2791,10 @@
         <v>1.954547571562129E-05</v>
       </c>
       <c r="K26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -2830,10 +2850,10 @@
         <v>0.001185098015687412</v>
       </c>
       <c r="K27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -2889,10 +2909,10 @@
         <v>3.147802341762763E-05</v>
       </c>
       <c r="K28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M28">
         <v>1</v>
@@ -2948,10 +2968,10 @@
         <v>1.36327821003782E-05</v>
       </c>
       <c r="K29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -3001,7 +3021,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3017,7 +3037,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3043,7 +3063,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3064,90 +3084,90 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -3167,25 +3187,25 @@
         <v>5</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>16</v>
@@ -3194,13 +3214,13 @@
         <v>20</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>7</v>
@@ -3211,34 +3231,34 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24">
-        <v>1.061036348342896</v>
+        <v>1.065426707267761</v>
       </c>
       <c r="B24">
-        <v>1.060370922088623</v>
+        <v>1.064475774765015</v>
       </c>
       <c r="C24">
-        <v>1.060013651847839</v>
+        <v>1.063900113105774</v>
       </c>
       <c r="D24">
-        <v>1.059879660606384</v>
+        <v>1.063494324684143</v>
       </c>
       <c r="E24">
-        <v>1.059901714324951</v>
+        <v>1.063193678855896</v>
       </c>
       <c r="F24">
-        <v>1.061036348342896</v>
+        <v>1.065426707267761</v>
       </c>
       <c r="G24">
         <v>1.05737</v>
       </c>
       <c r="H24">
-        <v>-0.003666348342895587</v>
+        <v>-0.008056707267761309</v>
       </c>
       <c r="I24">
-        <v>0.003666348342895587</v>
+        <v>0.008056707267761309</v>
       </c>
       <c r="J24">
-        <v>1.344211017145321E-05</v>
+        <v>6.49105319983979E-05</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -3264,40 +3284,40 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25">
-        <v>1.101883411407471</v>
+        <v>1.101836562156677</v>
       </c>
       <c r="B25">
-        <v>1.101805090904236</v>
+        <v>1.101790428161621</v>
       </c>
       <c r="C25">
-        <v>1.101748704910278</v>
+        <v>1.101749420166016</v>
       </c>
       <c r="D25">
-        <v>1.101709961891174</v>
+        <v>1.101714491844177</v>
       </c>
       <c r="E25">
-        <v>1.101683497428894</v>
+        <v>1.101683378219604</v>
       </c>
       <c r="F25">
-        <v>1.101883411407471</v>
+        <v>1.101836562156677</v>
       </c>
       <c r="G25">
         <v>1.09597</v>
       </c>
       <c r="H25">
-        <v>-0.005913411407470814</v>
+        <v>-0.005866562156677357</v>
       </c>
       <c r="I25">
-        <v>0.005913411407470814</v>
+        <v>0.005866562156677357</v>
       </c>
       <c r="J25">
-        <v>3.496843447400596E-05</v>
+        <v>3.441655153815888E-05</v>
       </c>
       <c r="K25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -3323,40 +3343,40 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26">
-        <v>1.118232488632202</v>
+        <v>1.119994044303894</v>
       </c>
       <c r="B26">
-        <v>1.121568083763123</v>
+        <v>1.12272310256958</v>
       </c>
       <c r="C26">
-        <v>1.12369441986084</v>
+        <v>1.124536037445068</v>
       </c>
       <c r="D26">
-        <v>1.124985218048096</v>
+        <v>1.125718832015991</v>
       </c>
       <c r="E26">
-        <v>1.125717520713806</v>
+        <v>1.126471757888794</v>
       </c>
       <c r="F26">
-        <v>1.118232488632202</v>
+        <v>1.119994044303894</v>
       </c>
       <c r="G26">
         <v>1.12275</v>
       </c>
       <c r="H26">
-        <v>0.004517511367797766</v>
+        <v>0.002755955696105872</v>
       </c>
       <c r="I26">
-        <v>0.004517511367797766</v>
+        <v>0.002755955696105872</v>
       </c>
       <c r="J26">
-        <v>2.040790895818204E-05</v>
+        <v>7.5952917988984E-06</v>
       </c>
       <c r="K26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -3382,40 +3402,40 @@
     </row>
     <row r="27" spans="1:19">
       <c r="A27">
-        <v>1.063446283340454</v>
+        <v>1.063027620315552</v>
       </c>
       <c r="B27">
-        <v>1.063025236129761</v>
+        <v>1.062199473381042</v>
       </c>
       <c r="C27">
-        <v>1.062759041786194</v>
+        <v>1.061497688293457</v>
       </c>
       <c r="D27">
-        <v>1.062629699707031</v>
+        <v>1.060908794403076</v>
       </c>
       <c r="E27">
-        <v>1.062600135803223</v>
+        <v>1.060402512550354</v>
       </c>
       <c r="F27">
-        <v>1.063446283340454</v>
+        <v>1.063027620315552</v>
       </c>
       <c r="G27">
         <v>1.05706</v>
       </c>
       <c r="H27">
-        <v>-0.006386283340454213</v>
+        <v>-0.005967620315551869</v>
       </c>
       <c r="I27">
-        <v>0.006386283340454213</v>
+        <v>0.005967620315551869</v>
       </c>
       <c r="J27">
-        <v>4.078461490456302E-05</v>
+        <v>3.561249223058739E-05</v>
       </c>
       <c r="K27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -3441,40 +3461,40 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28">
-        <v>1.090118169784546</v>
+        <v>1.08881676197052</v>
       </c>
       <c r="B28">
-        <v>1.088535785675049</v>
+        <v>1.087397694587708</v>
       </c>
       <c r="C28">
-        <v>1.08747661113739</v>
+        <v>1.086368560791016</v>
       </c>
       <c r="D28">
-        <v>1.086775779724121</v>
+        <v>1.085638523101807</v>
       </c>
       <c r="E28">
-        <v>1.086311101913452</v>
+        <v>1.08512282371521</v>
       </c>
       <c r="F28">
-        <v>1.090118169784546</v>
+        <v>1.08881676197052</v>
       </c>
       <c r="G28">
         <v>1.07974</v>
       </c>
       <c r="H28">
-        <v>-0.01037816978454598</v>
+        <v>-0.009076761970520097</v>
       </c>
       <c r="I28">
-        <v>0.01037816978454598</v>
+        <v>0.009076761970520097</v>
       </c>
       <c r="J28">
-        <v>0.0001077064080768631</v>
+        <v>8.238760786947989E-05</v>
       </c>
       <c r="K28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M28">
         <v>1</v>
@@ -3500,40 +3520,40 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29">
-        <v>1.073845624923706</v>
+        <v>1.074874639511108</v>
       </c>
       <c r="B29">
-        <v>1.073388576507568</v>
+        <v>1.074644923210144</v>
       </c>
       <c r="C29">
-        <v>1.073067903518677</v>
+        <v>1.074638485908508</v>
       </c>
       <c r="D29">
-        <v>1.072847723960876</v>
+        <v>1.074784159660339</v>
       </c>
       <c r="E29">
-        <v>1.072694063186646</v>
+        <v>1.075030207633972</v>
       </c>
       <c r="F29">
-        <v>1.073845624923706</v>
+        <v>1.074874639511108</v>
       </c>
       <c r="G29">
         <v>1.07728</v>
       </c>
       <c r="H29">
-        <v>0.003434375076293961</v>
+        <v>0.002405360488891617</v>
       </c>
       <c r="I29">
-        <v>0.003434375076293961</v>
+        <v>0.002405360488891617</v>
       </c>
       <c r="J29">
-        <v>1.179493216466915E-05</v>
+        <v>5.785759081520918E-06</v>
       </c>
       <c r="K29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -3559,40 +3579,40 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30">
-        <v>1.06854236125946</v>
+        <v>1.068402647972107</v>
       </c>
       <c r="B30">
-        <v>1.069087862968445</v>
+        <v>1.069523811340332</v>
       </c>
       <c r="C30">
-        <v>1.069251179695129</v>
+        <v>1.070211291313171</v>
       </c>
       <c r="D30">
-        <v>1.06916332244873</v>
+        <v>1.070587635040283</v>
       </c>
       <c r="E30">
-        <v>1.068921566009521</v>
+        <v>1.070764660835266</v>
       </c>
       <c r="F30">
-        <v>1.06854236125946</v>
+        <v>1.068402647972107</v>
       </c>
       <c r="G30">
         <v>1.07297</v>
       </c>
       <c r="H30">
-        <v>0.00442763874053953</v>
+        <v>0.004567352027893046</v>
       </c>
       <c r="I30">
-        <v>0.00442763874053953</v>
+        <v>0.004567352027893046</v>
       </c>
       <c r="J30">
-        <v>1.960398481672648E-05</v>
+        <v>2.086070454669872E-05</v>
       </c>
       <c r="K30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -3618,40 +3638,40 @@
     </row>
     <row r="31" spans="1:19">
       <c r="A31">
-        <v>1.076687812805176</v>
+        <v>1.075363278388977</v>
       </c>
       <c r="B31">
-        <v>1.077962279319763</v>
+        <v>1.076147437095642</v>
       </c>
       <c r="C31">
-        <v>1.078991055488586</v>
+        <v>1.076534152030945</v>
       </c>
       <c r="D31">
-        <v>1.079822659492493</v>
+        <v>1.076644659042358</v>
       </c>
       <c r="E31">
-        <v>1.080508470535278</v>
+        <v>1.076587796211243</v>
       </c>
       <c r="F31">
-        <v>1.076687812805176</v>
+        <v>1.075363278388977</v>
       </c>
       <c r="G31">
         <v>1.0811</v>
       </c>
       <c r="H31">
-        <v>0.004412187194824169</v>
+        <v>0.005736721611022899</v>
       </c>
       <c r="I31">
-        <v>0.004412187194824169</v>
+        <v>0.005736721611022899</v>
       </c>
       <c r="J31">
-        <v>1.946739584217037E-05</v>
+        <v>3.290997484237717E-05</v>
       </c>
       <c r="K31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M31">
         <v>1</v>
@@ -3677,40 +3697,40 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32">
-        <v>1.102351903915405</v>
+        <v>1.101925253868103</v>
       </c>
       <c r="B32">
-        <v>1.101625919342041</v>
+        <v>1.100845098495483</v>
       </c>
       <c r="C32">
-        <v>1.101073503494263</v>
+        <v>1.100005388259888</v>
       </c>
       <c r="D32">
-        <v>1.100651025772095</v>
+        <v>1.099330067634583</v>
       </c>
       <c r="E32">
-        <v>1.100320219993591</v>
+        <v>1.098767876625061</v>
       </c>
       <c r="F32">
-        <v>1.102351903915405</v>
+        <v>1.101925253868103</v>
       </c>
       <c r="G32">
         <v>1.10726</v>
       </c>
       <c r="H32">
-        <v>0.004908096084594638</v>
+        <v>0.005334746131896884</v>
       </c>
       <c r="I32">
-        <v>0.004908096084594638</v>
+        <v>0.005334746131896884</v>
       </c>
       <c r="J32">
-        <v>2.408940717561321E-05</v>
+        <v>2.845951629178876E-05</v>
       </c>
       <c r="K32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -3736,40 +3756,40 @@
     </row>
     <row r="33" spans="1:19">
       <c r="A33">
-        <v>1.057507157325745</v>
+        <v>1.05669379234314</v>
       </c>
       <c r="B33">
-        <v>1.057982325553894</v>
+        <v>1.056609988212585</v>
       </c>
       <c r="C33">
-        <v>1.058434128761292</v>
+        <v>1.056416630744934</v>
       </c>
       <c r="D33">
-        <v>1.058842539787292</v>
+        <v>1.056138038635254</v>
       </c>
       <c r="E33">
-        <v>1.059202075004578</v>
+        <v>1.055789589881897</v>
       </c>
       <c r="F33">
-        <v>1.057507157325745</v>
+        <v>1.05669379234314</v>
       </c>
       <c r="G33">
         <v>1.0472</v>
       </c>
       <c r="H33">
-        <v>-0.01030715732574472</v>
+        <v>-0.00949379234313974</v>
       </c>
       <c r="I33">
-        <v>0.01030715732574472</v>
+        <v>0.00949379234313974</v>
       </c>
       <c r="J33">
-        <v>0.0001062374921376531</v>
+        <v>9.013209305465876E-05</v>
       </c>
       <c r="K33" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L33" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M33">
         <v>1</v>
@@ -3795,40 +3815,40 @@
     </row>
     <row r="34" spans="1:19">
       <c r="A34">
-        <v>1.037141561508179</v>
+        <v>1.037492036819458</v>
       </c>
       <c r="B34">
-        <v>1.035979747772217</v>
+        <v>1.036292552947998</v>
       </c>
       <c r="C34">
-        <v>1.035399675369263</v>
+        <v>1.035528779029846</v>
       </c>
       <c r="D34">
-        <v>1.035161852836609</v>
+        <v>1.035053491592407</v>
       </c>
       <c r="E34">
-        <v>1.035085916519165</v>
+        <v>1.034741044044495</v>
       </c>
       <c r="F34">
-        <v>1.037141561508179</v>
+        <v>1.037492036819458</v>
       </c>
       <c r="G34">
         <v>1.03342</v>
       </c>
       <c r="H34">
-        <v>-0.003721561508178706</v>
+        <v>-0.004072036819458003</v>
       </c>
       <c r="I34">
-        <v>0.003721561508178706</v>
+        <v>0.004072036819458003</v>
       </c>
       <c r="J34">
-        <v>1.385002005915736E-05</v>
+        <v>1.658148385902165E-05</v>
       </c>
       <c r="K34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M34">
         <v>1</v>
@@ -3854,40 +3874,40 @@
     </row>
     <row r="35" spans="1:19">
       <c r="A35">
-        <v>1.117325186729431</v>
+        <v>1.117155075073242</v>
       </c>
       <c r="B35">
-        <v>1.121643900871277</v>
+        <v>1.120662450790405</v>
       </c>
       <c r="C35">
-        <v>1.123468518257141</v>
+        <v>1.12163770198822</v>
       </c>
       <c r="D35">
-        <v>1.123796224594116</v>
+        <v>1.121259927749634</v>
       </c>
       <c r="E35">
-        <v>1.123104572296143</v>
+        <v>1.119905591011047</v>
       </c>
       <c r="F35">
-        <v>1.117325186729431</v>
+        <v>1.117155075073242</v>
       </c>
       <c r="G35">
         <v>1.13503</v>
       </c>
       <c r="H35">
-        <v>0.01770481327056883</v>
+        <v>0.0178749249267578</v>
       </c>
       <c r="I35">
-        <v>0.01770481327056883</v>
+        <v>0.0178749249267578</v>
       </c>
       <c r="J35">
-        <v>0.0003134604129457102</v>
+        <v>0.0003195129411372272</v>
       </c>
       <c r="K35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M35">
         <v>1</v>
@@ -3913,40 +3933,40 @@
     </row>
     <row r="36" spans="1:19">
       <c r="A36">
-        <v>1.145053148269653</v>
+        <v>1.143898606300354</v>
       </c>
       <c r="B36">
-        <v>1.143314599990845</v>
+        <v>1.141653180122375</v>
       </c>
       <c r="C36">
-        <v>1.141129016876221</v>
+        <v>1.139041662216187</v>
       </c>
       <c r="D36">
-        <v>1.138800144195557</v>
+        <v>1.13631010055542</v>
       </c>
       <c r="E36">
-        <v>1.136436581611633</v>
+        <v>1.133596301078796</v>
       </c>
       <c r="F36">
-        <v>1.145053148269653</v>
+        <v>1.143898606300354</v>
       </c>
       <c r="G36">
         <v>1.15777</v>
       </c>
       <c r="H36">
-        <v>0.01271685173034665</v>
+        <v>0.01387139369964596</v>
       </c>
       <c r="I36">
-        <v>0.01271685173034665</v>
+        <v>0.01387139369964596</v>
       </c>
       <c r="J36">
-        <v>0.0001617183179316205</v>
+        <v>0.0001924155631705777</v>
       </c>
       <c r="K36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M36">
         <v>1</v>
@@ -3972,40 +3992,40 @@
     </row>
     <row r="37" spans="1:19">
       <c r="A37">
-        <v>1.163928031921387</v>
+        <v>1.167031764984131</v>
       </c>
       <c r="B37">
-        <v>1.163788080215454</v>
+        <v>1.167843818664551</v>
       </c>
       <c r="C37">
-        <v>1.163005828857422</v>
+        <v>1.168604850769043</v>
       </c>
       <c r="D37">
-        <v>1.161831021308899</v>
+        <v>1.169304132461548</v>
       </c>
       <c r="E37">
-        <v>1.160386443138123</v>
+        <v>1.16994309425354</v>
       </c>
       <c r="F37">
-        <v>1.163928031921387</v>
+        <v>1.167031764984131</v>
       </c>
       <c r="G37">
         <v>1.17117</v>
       </c>
       <c r="H37">
-        <v>0.007241968078613326</v>
+        <v>0.004138235015869185</v>
       </c>
       <c r="I37">
-        <v>0.007241968078613326</v>
+        <v>0.004138235015869185</v>
       </c>
       <c r="J37">
-        <v>5.244610165165438E-05</v>
+        <v>1.712498904656583E-05</v>
       </c>
       <c r="K37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M37">
         <v>1</v>
@@ -4036,7 +4056,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4044,7 +4064,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -4052,79 +4072,79 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -4132,7 +4152,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
@@ -4140,95 +4160,95 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
@@ -4236,98 +4256,114 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B25" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se añade la configuracion para que se haga el backtesting dinámico y escoja el mejor modelo segun un plantilla config_2.YAML o un grid
</commit_message>
<xml_diff>
--- a/outputs/backtest_plots/EURUSD_backtest_consolidado.xlsx
+++ b/outputs/backtest_plots/EURUSD_backtest_consolidado.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="209">
   <si>
     <t>model</t>
   </si>
@@ -95,7 +95,7 @@
     <t>param.seasonal</t>
   </si>
   <si>
-    <t>param.m</t>
+    <t>param.order</t>
   </si>
   <si>
     <t>param.modo</t>
@@ -125,39 +125,39 @@
     <t>param.enforce_invertibility</t>
   </si>
   <si>
-    <t>param.order</t>
-  </si>
-  <si>
     <t>EURUSD</t>
   </si>
   <si>
     <t>returns</t>
   </si>
   <si>
-    <t>fixed</t>
+    <t>atr</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>aic</t>
   </si>
   <si>
     <t>False</t>
   </si>
   <si>
-    <t>aic</t>
-  </si>
-  <si>
-    <t>12</t>
+    <t>[0, 1, 2]</t>
   </si>
   <si>
     <t>retornos</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>[0, 1, 2]</t>
-  </si>
-  <si>
     <t>y_pred</t>
   </si>
   <si>
@@ -206,7 +206,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>0.5</t>
+    <t>0.3</t>
   </si>
   <si>
     <t>multiplicative</t>
@@ -254,7 +254,7 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>40</t>
+    <t>60</t>
   </si>
   <si>
     <t>32</t>
@@ -272,15 +272,9 @@
     <t>standard</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>outputs/modelos/lstm</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>config_key</t>
   </si>
   <si>
@@ -311,27 +305,6 @@
     <t>eda.frecuencia_resampleo</t>
   </si>
   <si>
-    <t>modelo.nombre</t>
-  </si>
-  <si>
-    <t>modelo.objetivo</t>
-  </si>
-  <si>
-    <t>modelo.horizonte</t>
-  </si>
-  <si>
-    <t>modelo.params.order</t>
-  </si>
-  <si>
-    <t>modelo.params.seasonal_order</t>
-  </si>
-  <si>
-    <t>modelo.params.enforce_stationarity</t>
-  </si>
-  <si>
-    <t>modelo.params.enforce_invertibility</t>
-  </si>
-  <si>
     <t>validacion.modo</t>
   </si>
   <si>
@@ -380,6 +353,9 @@
     <t>bt.log_threshold_used</t>
   </si>
   <si>
+    <t>bt.auto.scan.thresholds</t>
+  </si>
+  <si>
     <t>bt.auto.rescan_each_refit</t>
   </si>
   <si>
@@ -539,9 +515,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>[0, 0, 0, 0]</t>
-  </si>
-  <si>
     <t>last_n</t>
   </si>
   <si>
@@ -551,73 +524,82 @@
     <t>20</t>
   </si>
   <si>
-    <t>[{'name': 'ARIMA', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'auto': False, 'metric': 'aic', 'seasonal': False, 'm': 12, 'modo': 'retornos', 'max_p': 2, 'max_q': 2, 'max_P': 2, 'max_Q': 2, 'max_d': 2, 'max_D': 1, 'enforce_stationarity': False, 'enforce_invertibility': False, 'order': [0, 1, 2]}, 'normal': {}, 'backtest': {'engine': 'model'}}, {'name': 'RW', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'order': [0, 1, 0], 'seasonal_order': [0, 0, 0, 0], 'enforce_stationarity': False, 'enforce_invertibility': False}, 'normal': {}, 'backtest': {'engine': 'classic_auto'}}, {'name': 'PROPHET', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'frequency_hint': 'D1', 'changepoint_prior_scale': 0.5, 'seasonality_mode': 'multiplicative'}, 'normal': {}, 'backtest': {'engine': 'model', 'prophet': {'frequency_hint': 'D1', 'yearly_seasonality': False, 'weekly_seasonality': True, 'daily_seasonality': True, 'interval_width': 0.9}}}, {'name': 'LSTM', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'window': 64, 'units': 64, 'dropout': 0.2, 'epochs': 40, 'batch_size': 32, 'lr': 0.001, 'loss': 'mse', 'optimizer': 'adam', 'scaler': 'standard', 'patience': 5, 'model_dir': 'outputs/modelos/lstm', 'reuse_pretrained': True}, 'normal': {}, 'backtest': {'engine': 'model', 'lstm': {'horizon': 5}}}]</t>
+    <t>[{'name': 'ARIMA', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'auto': True, 'metric': 'aic', 'seasonal': False, 'order': [0, 1, 2], 'modo': 'retornos', 'max_p': 5, 'max_q': 5, 'max_P': 2, 'max_Q': 2, 'max_d': 2, 'max_D': 1, 'enforce_stationarity': False, 'enforce_invertibility': False}, 'normal': {}, 'backtest': {'engine': 'classic_auto'}}, {'name': 'RW', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'order': [0, 1, 0], 'seasonal_order': [0, 0, 0, 0], 'enforce_stationarity': False, 'enforce_invertibility': False}, 'normal': {}, 'backtest': {'engine': 'classic_auto'}}, {'name': 'PROPHET', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'frequency_hint': 'D1', 'changepoint_prior_scale': 0.3, 'seasonality_mode': 'multiplicative'}, 'normal': {}, 'backtest': {'engine': 'model', 'prophet': {'frequency_hint': 'D1', 'yearly_seasonality': False, 'weekly_seasonality': True, 'daily_seasonality': True, 'interval_width': 0.8}}}, {'name': 'LSTM', 'enabled': True, 'objetivo': 'retornos', 'horizonte': 5, 'params': {'window': 64, 'units': 64, 'dropout': 0.2, 'epochs': 60, 'batch_size': 32, 'lr': 0.001, 'loss': 'mse', 'optimizer': 'adam', 'scaler': 'standard', 'patience': 5, 'model_dir': 'outputs/modelos/lstm', 'reuse_pretrained': True}, 'normal': {}, 'backtest': {'engine': 'model', 'lstm': {'horizon': 1}}}]</t>
   </si>
   <si>
     <t>800</t>
   </si>
   <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>[8, 10, 12, 14]</t>
+  </si>
+  <si>
+    <t>999999</t>
+  </si>
+  <si>
+    <t>[1, 2, 3]</t>
+  </si>
+  <si>
+    <t>outputs/evaluacion.xlsx</t>
+  </si>
+  <si>
+    <t>outputs/backtest_plots</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>logs/marki.log</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>['D1']</t>
+  </si>
+  <si>
+    <t>['D', 'H']</t>
+  </si>
+  <si>
+    <t>['retornos', 'precio']</t>
+  </si>
+  <si>
+    <t>['returns', 'price']</t>
+  </si>
+  <si>
+    <t>['last_n', 'date_range']</t>
+  </si>
+  <si>
+    <t>['model', 'classic_auto']</t>
+  </si>
+  <si>
+    <t>['adam', 'sgd', 'rmsprop', 'adagrad', 'adamw']</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
     <t>50</t>
-  </si>
-  <si>
-    <t>0.0001</t>
-  </si>
-  <si>
-    <t>12.0</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>999999</t>
-  </si>
-  <si>
-    <t>[1, 2, 3]</t>
-  </si>
-  <si>
-    <t>outputs/evaluacion.xlsx</t>
-  </si>
-  <si>
-    <t>outputs/backtest_plots</t>
-  </si>
-  <si>
-    <t>INFO</t>
-  </si>
-  <si>
-    <t>logs/marki.log</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>['D1']</t>
-  </si>
-  <si>
-    <t>['D', 'H']</t>
-  </si>
-  <si>
-    <t>['retornos', 'precio']</t>
-  </si>
-  <si>
-    <t>['returns', 'price']</t>
-  </si>
-  <si>
-    <t>['last_n', 'date_range']</t>
-  </si>
-  <si>
-    <t>['model', 'classic_auto']</t>
-  </si>
-  <si>
-    <t>['adam', 'sgd', 'rmsprop', 'adagrad', 'adamw']</t>
-  </si>
-  <si>
-    <t>50000</t>
   </si>
   <si>
     <t>5000</t>
@@ -1064,25 +1046,25 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0.002815000000000123</v>
+        <v>0.004045000000000021</v>
       </c>
       <c r="C2">
-        <v>0.003066944733770187</v>
+        <v>0.004881577613845766</v>
       </c>
       <c r="D2">
-        <v>0.002609005344946002</v>
+        <v>0.003759384026729092</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>536.8947282345351</v>
+        <v>748.4747251303345</v>
       </c>
       <c r="H2" s="2">
-        <v>43864</v>
+        <v>43865</v>
       </c>
       <c r="I2" s="2">
-        <v>44985</v>
+        <v>44986</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1090,25 +1072,25 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0.0145133910199417</v>
+        <v>0.01091318068476876</v>
       </c>
       <c r="C3">
-        <v>0.01628552178890887</v>
+        <v>0.01240310214696966</v>
       </c>
       <c r="D3">
-        <v>0.01328425899546071</v>
+        <v>0.01006154517020638</v>
       </c>
       <c r="E3">
-        <v>0.6666666666666666</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G3">
-        <v>536.8947282345351</v>
+        <v>748.4747251303345</v>
       </c>
       <c r="H3" s="2">
-        <v>43864</v>
+        <v>43865</v>
       </c>
       <c r="I3" s="2">
-        <v>44985</v>
+        <v>44986</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1116,25 +1098,25 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.00595475759506231</v>
+        <v>0.004052407984733608</v>
       </c>
       <c r="C4">
-        <v>0.006355317250576697</v>
+        <v>0.005855432879047838</v>
       </c>
       <c r="D4">
-        <v>0.005461627164110089</v>
+        <v>0.003791010934179465</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="G4">
-        <v>536.8947282345351</v>
+        <v>748.4747251303345</v>
       </c>
       <c r="H4" s="2">
-        <v>43864</v>
+        <v>43865</v>
       </c>
       <c r="I4" s="2">
-        <v>44985</v>
+        <v>44986</v>
       </c>
     </row>
   </sheetData>
@@ -1144,7 +1126,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1163,7 +1145,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1179,7 +1161,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1205,7 +1187,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1229,7 +1211,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1237,7 +1219,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1245,7 +1227,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1285,7 +1267,7 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1293,7 +1275,7 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -1301,7 +1283,7 @@
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -1309,7 +1291,7 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -1317,7 +1299,7 @@
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -1325,106 +1307,157 @@
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="1">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="1">
-        <v>1</v>
-      </c>
-      <c r="B26" s="1">
-        <v>2</v>
-      </c>
-      <c r="C26" s="1">
-        <v>3</v>
-      </c>
-      <c r="D26" s="1">
-        <v>4</v>
-      </c>
-      <c r="E26" s="1">
-        <v>5</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>8</v>
+      <c r="A26">
+        <v>1.05737</v>
+      </c>
+      <c r="B26">
+        <v>1.05737</v>
+      </c>
+      <c r="C26">
+        <v>1.05737</v>
+      </c>
+      <c r="D26">
+        <v>1.05737</v>
+      </c>
+      <c r="E26">
+        <v>1.05737</v>
+      </c>
+      <c r="F26">
+        <v>1.05737</v>
+      </c>
+      <c r="G26">
+        <v>1.06686</v>
+      </c>
+      <c r="H26">
+        <v>0.009489999999999998</v>
+      </c>
+      <c r="I26">
+        <v>0.009489999999999998</v>
+      </c>
+      <c r="J26">
+        <v>9.006009999999997E-05</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>12</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1.06686</v>
+      </c>
+      <c r="Q26">
+        <v>1.06686</v>
+      </c>
+      <c r="R26" s="2">
+        <v>43865</v>
+      </c>
+      <c r="S26" s="2">
+        <v>44986</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27">
-        <v>1.06089</v>
+        <v>1.09552</v>
       </c>
       <c r="B27">
-        <v>1.06089</v>
+        <v>1.09552</v>
       </c>
       <c r="C27">
-        <v>1.06089</v>
+        <v>1.09552</v>
       </c>
       <c r="D27">
-        <v>1.06089</v>
+        <v>1.09552</v>
       </c>
       <c r="E27">
-        <v>1.06089</v>
+        <v>1.09552</v>
       </c>
       <c r="F27">
-        <v>1.06089</v>
+        <v>1.09552</v>
       </c>
       <c r="G27">
-        <v>1.05737</v>
+        <v>1.09051</v>
       </c>
       <c r="H27">
-        <v>-0.00352000000000019</v>
+        <v>-0.005009999999999959</v>
       </c>
       <c r="I27">
-        <v>0.00352000000000019</v>
+        <v>0.005009999999999959</v>
       </c>
       <c r="J27">
-        <v>1.239040000000134E-05</v>
+        <v>2.510009999999959E-05</v>
+      </c>
+      <c r="K27" t="s">
+        <v>56</v>
+      </c>
+      <c r="L27" t="s">
+        <v>56</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -1436,48 +1469,48 @@
         <v>1</v>
       </c>
       <c r="P27">
-        <v>1.05737</v>
+        <v>1.09051</v>
       </c>
       <c r="Q27">
-        <v>1.05737</v>
+        <v>2.15737</v>
       </c>
       <c r="R27" s="2">
-        <v>43864</v>
+        <v>43900</v>
       </c>
       <c r="S27" s="2">
-        <v>44985</v>
+        <v>45021</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28">
-        <v>1.10035</v>
+        <v>1.09597</v>
       </c>
       <c r="B28">
-        <v>1.10035</v>
+        <v>1.09597</v>
       </c>
       <c r="C28">
-        <v>1.10035</v>
+        <v>1.09597</v>
       </c>
       <c r="D28">
-        <v>1.10035</v>
+        <v>1.09597</v>
       </c>
       <c r="E28">
-        <v>1.10035</v>
+        <v>1.09597</v>
       </c>
       <c r="F28">
-        <v>1.10035</v>
+        <v>1.09597</v>
       </c>
       <c r="G28">
-        <v>1.09597</v>
+        <v>1.09826</v>
       </c>
       <c r="H28">
-        <v>-0.004380000000000051</v>
+        <v>0.002290000000000125</v>
       </c>
       <c r="I28">
-        <v>0.004380000000000051</v>
+        <v>0.002290000000000125</v>
       </c>
       <c r="J28">
-        <v>1.918440000000044E-05</v>
+        <v>5.244100000000574E-06</v>
       </c>
       <c r="K28" t="s">
         <v>56</v>
@@ -1495,54 +1528,54 @@
         <v>1</v>
       </c>
       <c r="P28">
-        <v>1.09597</v>
+        <v>1.09826</v>
       </c>
       <c r="Q28">
-        <v>2.15334</v>
+        <v>3.25563</v>
       </c>
       <c r="R28" s="2">
-        <v>43934</v>
+        <v>43935</v>
       </c>
       <c r="S28" s="2">
-        <v>45055</v>
+        <v>45056</v>
       </c>
     </row>
     <row r="29" spans="1:19">
       <c r="A29">
-        <v>1.12398</v>
+        <v>1.07916</v>
       </c>
       <c r="B29">
-        <v>1.12398</v>
+        <v>1.07916</v>
       </c>
       <c r="C29">
-        <v>1.12398</v>
+        <v>1.07916</v>
       </c>
       <c r="D29">
-        <v>1.12398</v>
+        <v>1.07916</v>
       </c>
       <c r="E29">
-        <v>1.12398</v>
+        <v>1.07916</v>
       </c>
       <c r="F29">
-        <v>1.12398</v>
+        <v>1.07916</v>
       </c>
       <c r="G29">
-        <v>1.12275</v>
+        <v>1.08305</v>
       </c>
       <c r="H29">
-        <v>-0.001230000000000064</v>
+        <v>0.003890000000000171</v>
       </c>
       <c r="I29">
-        <v>0.001230000000000064</v>
+        <v>0.003890000000000171</v>
       </c>
       <c r="J29">
-        <v>1.512900000000158E-06</v>
+        <v>1.513210000000133E-05</v>
       </c>
       <c r="K29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -1554,54 +1587,54 @@
         <v>1</v>
       </c>
       <c r="P29">
-        <v>1.12275</v>
+        <v>1.08305</v>
       </c>
       <c r="Q29">
-        <v>3.27609</v>
+        <v>4.33868</v>
       </c>
       <c r="R29" s="2">
-        <v>44004</v>
+        <v>43970</v>
       </c>
       <c r="S29" s="2">
-        <v>45125</v>
+        <v>45091</v>
       </c>
     </row>
     <row r="30" spans="1:19">
       <c r="A30">
-        <v>1.05919</v>
+        <v>1.12275</v>
       </c>
       <c r="B30">
-        <v>1.05919</v>
+        <v>1.12275</v>
       </c>
       <c r="C30">
-        <v>1.05919</v>
+        <v>1.12275</v>
       </c>
       <c r="D30">
-        <v>1.05919</v>
+        <v>1.12275</v>
       </c>
       <c r="E30">
-        <v>1.05919</v>
+        <v>1.12275</v>
       </c>
       <c r="F30">
-        <v>1.05919</v>
+        <v>1.12275</v>
       </c>
       <c r="G30">
-        <v>1.05706</v>
+        <v>1.12012</v>
       </c>
       <c r="H30">
-        <v>-0.002130000000000187</v>
+        <v>-0.00262999999999991</v>
       </c>
       <c r="I30">
-        <v>0.002130000000000187</v>
+        <v>0.00262999999999991</v>
       </c>
       <c r="J30">
-        <v>4.536900000000798E-06</v>
+        <v>6.916899999999528E-06</v>
       </c>
       <c r="K30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -1613,16 +1646,193 @@
         <v>1</v>
       </c>
       <c r="P30">
+        <v>1.12012</v>
+      </c>
+      <c r="Q30">
+        <v>5.4588</v>
+      </c>
+      <c r="R30" s="2">
+        <v>44005</v>
+      </c>
+      <c r="S30" s="2">
+        <v>45126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31">
+        <v>1.08465</v>
+      </c>
+      <c r="B31">
+        <v>1.08465</v>
+      </c>
+      <c r="C31">
+        <v>1.08465</v>
+      </c>
+      <c r="D31">
+        <v>1.08465</v>
+      </c>
+      <c r="E31">
+        <v>1.08465</v>
+      </c>
+      <c r="F31">
+        <v>1.08465</v>
+      </c>
+      <c r="G31">
+        <v>1.08628</v>
+      </c>
+      <c r="H31">
+        <v>0.00163000000000002</v>
+      </c>
+      <c r="I31">
+        <v>0.00163000000000002</v>
+      </c>
+      <c r="J31">
+        <v>2.656900000000066E-06</v>
+      </c>
+      <c r="K31" t="s">
+        <v>57</v>
+      </c>
+      <c r="L31" t="s">
+        <v>57</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>12</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1.08628</v>
+      </c>
+      <c r="Q31">
+        <v>6.54508</v>
+      </c>
+      <c r="R31" s="2">
+        <v>44040</v>
+      </c>
+      <c r="S31" s="2">
+        <v>45161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32">
         <v>1.05706</v>
       </c>
-      <c r="Q30">
-        <v>4.33315</v>
-      </c>
-      <c r="R30" s="2">
-        <v>44074</v>
-      </c>
-      <c r="S30" s="2">
-        <v>45195</v>
+      <c r="B32">
+        <v>1.05706</v>
+      </c>
+      <c r="C32">
+        <v>1.05706</v>
+      </c>
+      <c r="D32">
+        <v>1.05706</v>
+      </c>
+      <c r="E32">
+        <v>1.05706</v>
+      </c>
+      <c r="F32">
+        <v>1.05706</v>
+      </c>
+      <c r="G32">
+        <v>1.05035</v>
+      </c>
+      <c r="H32">
+        <v>-0.006709999999999994</v>
+      </c>
+      <c r="I32">
+        <v>0.006709999999999994</v>
+      </c>
+      <c r="J32">
+        <v>4.502409999999991E-05</v>
+      </c>
+      <c r="K32" t="s">
+        <v>57</v>
+      </c>
+      <c r="L32" t="s">
+        <v>57</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>12</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>1.05035</v>
+      </c>
+      <c r="Q32">
+        <v>7.59543</v>
+      </c>
+      <c r="R32" s="2">
+        <v>44075</v>
+      </c>
+      <c r="S32" s="2">
+        <v>45196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33">
+        <v>1.05732</v>
+      </c>
+      <c r="B33">
+        <v>1.05732</v>
+      </c>
+      <c r="C33">
+        <v>1.05732</v>
+      </c>
+      <c r="D33">
+        <v>1.05732</v>
+      </c>
+      <c r="E33">
+        <v>1.05732</v>
+      </c>
+      <c r="F33">
+        <v>1.05732</v>
+      </c>
+      <c r="G33">
+        <v>1.05661</v>
+      </c>
+      <c r="H33">
+        <v>-0.0007099999999999884</v>
+      </c>
+      <c r="I33">
+        <v>0.0007099999999999884</v>
+      </c>
+      <c r="J33">
+        <v>5.040999999999836E-07</v>
+      </c>
+      <c r="K33" t="s">
+        <v>56</v>
+      </c>
+      <c r="L33" t="s">
+        <v>56</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>12</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>1.05661</v>
+      </c>
+      <c r="Q33">
+        <v>8.65204</v>
+      </c>
+      <c r="R33" s="2">
+        <v>44110</v>
+      </c>
+      <c r="S33" s="2">
+        <v>45231</v>
       </c>
     </row>
   </sheetData>
@@ -1632,7 +1842,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1651,7 +1861,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1667,7 +1877,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1693,7 +1903,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -1797,34 +2007,34 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16">
-        <v>1.068349247873367</v>
+        <v>1.066906965638435</v>
       </c>
       <c r="B16">
-        <v>1.068154121467403</v>
+        <v>1.066586220361642</v>
       </c>
       <c r="C16">
-        <v>1.067911466914082</v>
+        <v>1.06620982955082</v>
       </c>
       <c r="D16">
-        <v>1.067610187344473</v>
+        <v>1.065767982331096</v>
       </c>
       <c r="E16">
-        <v>1.067240121144259</v>
+        <v>1.065252000418757</v>
       </c>
       <c r="F16">
-        <v>1.068349247873367</v>
+        <v>1.066906965638435</v>
       </c>
       <c r="G16">
-        <v>1.05737</v>
+        <v>1.06686</v>
       </c>
       <c r="H16">
-        <v>-0.01097924787336679</v>
+        <v>-4.696563843520352E-05</v>
       </c>
       <c r="I16">
-        <v>0.01097924787336679</v>
+        <v>4.696563843520352E-05</v>
       </c>
       <c r="J16">
-        <v>0.0001205438838648293</v>
+        <v>2.205771193626266E-09</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -1836,48 +2046,48 @@
         <v>1</v>
       </c>
       <c r="P16">
-        <v>1.05737</v>
+        <v>1.06686</v>
       </c>
       <c r="Q16">
-        <v>1.05737</v>
+        <v>1.06686</v>
       </c>
       <c r="R16" s="2">
-        <v>43864</v>
+        <v>43865</v>
       </c>
       <c r="S16" s="2">
-        <v>44985</v>
+        <v>44986</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17">
-        <v>1.104263081884899</v>
+        <v>1.079608762777349</v>
       </c>
       <c r="B17">
-        <v>1.105336399989389</v>
+        <v>1.080381647562092</v>
       </c>
       <c r="C17">
-        <v>1.106523344972875</v>
+        <v>1.081144302982017</v>
       </c>
       <c r="D17">
-        <v>1.107821858140857</v>
+        <v>1.08188964988042</v>
       </c>
       <c r="E17">
-        <v>1.10922810353222</v>
+        <v>1.082610733709016</v>
       </c>
       <c r="F17">
-        <v>1.104263081884899</v>
+        <v>1.079608762777349</v>
       </c>
       <c r="G17">
-        <v>1.09597</v>
+        <v>1.09051</v>
       </c>
       <c r="H17">
-        <v>-0.008293081884899411</v>
+        <v>0.01090123722265157</v>
       </c>
       <c r="I17">
-        <v>0.008293081884899411</v>
+        <v>0.01090123722265157</v>
       </c>
       <c r="J17">
-        <v>6.877520714964678E-05</v>
+        <v>0.0001188369729845242</v>
       </c>
       <c r="K17" t="s">
         <v>56</v>
@@ -1895,54 +2105,54 @@
         <v>1</v>
       </c>
       <c r="P17">
-        <v>1.09597</v>
+        <v>1.09051</v>
       </c>
       <c r="Q17">
-        <v>2.15334</v>
+        <v>2.15737</v>
       </c>
       <c r="R17" s="2">
-        <v>43934</v>
+        <v>43900</v>
       </c>
       <c r="S17" s="2">
-        <v>45055</v>
+        <v>45021</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18">
-        <v>1.095627574480785</v>
+        <v>1.104278144111826</v>
       </c>
       <c r="B18">
-        <v>1.096644851664386</v>
+        <v>1.105376354584669</v>
       </c>
       <c r="C18">
-        <v>1.097725132174214</v>
+        <v>1.106588563574856</v>
       </c>
       <c r="D18">
-        <v>1.098858127852395</v>
+        <v>1.107911595511421</v>
       </c>
       <c r="E18">
-        <v>1.100032423843403</v>
+        <v>1.109340463362188</v>
       </c>
       <c r="F18">
-        <v>1.095627574480785</v>
+        <v>1.104278144111826</v>
       </c>
       <c r="G18">
-        <v>1.12275</v>
+        <v>1.09826</v>
       </c>
       <c r="H18">
-        <v>0.02712242551921529</v>
+        <v>-0.006018144111826107</v>
       </c>
       <c r="I18">
-        <v>0.02712242551921529</v>
+        <v>0.006018144111826107</v>
       </c>
       <c r="J18">
-        <v>0.0007356259660453807</v>
+        <v>3.621805855070724E-05</v>
       </c>
       <c r="K18" t="s">
         <v>56</v>
       </c>
       <c r="L18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -1954,48 +2164,48 @@
         <v>1</v>
       </c>
       <c r="P18">
-        <v>1.12275</v>
+        <v>1.09826</v>
       </c>
       <c r="Q18">
-        <v>3.27609</v>
+        <v>3.25563</v>
       </c>
       <c r="R18" s="2">
-        <v>44004</v>
+        <v>43935</v>
       </c>
       <c r="S18" s="2">
-        <v>45125</v>
+        <v>45056</v>
       </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19">
-        <v>1.068718808802285</v>
+        <v>1.072893710212931</v>
       </c>
       <c r="B19">
-        <v>1.068134688220237</v>
+        <v>1.071474456857362</v>
       </c>
       <c r="C19">
-        <v>1.067630928745228</v>
+        <v>1.069967528152536</v>
       </c>
       <c r="D19">
-        <v>1.067217357747553</v>
+        <v>1.068376785056323</v>
       </c>
       <c r="E19">
-        <v>1.066902506528437</v>
+        <v>1.066707024512989</v>
       </c>
       <c r="F19">
-        <v>1.068718808802285</v>
+        <v>1.072893710212931</v>
       </c>
       <c r="G19">
-        <v>1.05706</v>
+        <v>1.08305</v>
       </c>
       <c r="H19">
-        <v>-0.01165880880228531</v>
+        <v>0.01015628978706884</v>
       </c>
       <c r="I19">
-        <v>0.01165880880228531</v>
+        <v>0.01015628978706884</v>
       </c>
       <c r="J19">
-        <v>0.0001359278226882455</v>
+        <v>0.0001031502222389188</v>
       </c>
       <c r="K19" t="s">
         <v>57</v>
@@ -2013,16 +2223,252 @@
         <v>1</v>
       </c>
       <c r="P19">
-        <v>1.05706</v>
+        <v>1.08305</v>
       </c>
       <c r="Q19">
-        <v>4.33315</v>
+        <v>4.33868</v>
       </c>
       <c r="R19" s="2">
-        <v>44074</v>
+        <v>43970</v>
       </c>
       <c r="S19" s="2">
-        <v>45195</v>
+        <v>45091</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20">
+        <v>1.099623955415088</v>
+      </c>
+      <c r="B20">
+        <v>1.100790976100368</v>
+      </c>
+      <c r="C20">
+        <v>1.102000926885872</v>
+      </c>
+      <c r="D20">
+        <v>1.103242157930367</v>
+      </c>
+      <c r="E20">
+        <v>1.104502330336207</v>
+      </c>
+      <c r="F20">
+        <v>1.099623955415088</v>
+      </c>
+      <c r="G20">
+        <v>1.12012</v>
+      </c>
+      <c r="H20">
+        <v>0.02049604458491228</v>
+      </c>
+      <c r="I20">
+        <v>0.02049604458491228</v>
+      </c>
+      <c r="J20">
+        <v>0.0004200878436267119</v>
+      </c>
+      <c r="K20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>12</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1.12012</v>
+      </c>
+      <c r="Q20">
+        <v>5.4588</v>
+      </c>
+      <c r="R20" s="2">
+        <v>44005</v>
+      </c>
+      <c r="S20" s="2">
+        <v>45126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21">
+        <v>1.100108123350862</v>
+      </c>
+      <c r="B21">
+        <v>1.1007229990243</v>
+      </c>
+      <c r="C21">
+        <v>1.101398654075788</v>
+      </c>
+      <c r="D21">
+        <v>1.102128128574317</v>
+      </c>
+      <c r="E21">
+        <v>1.102903047148774</v>
+      </c>
+      <c r="F21">
+        <v>1.100108123350862</v>
+      </c>
+      <c r="G21">
+        <v>1.08628</v>
+      </c>
+      <c r="H21">
+        <v>-0.01382812335086192</v>
+      </c>
+      <c r="I21">
+        <v>0.01382812335086192</v>
+      </c>
+      <c r="J21">
+        <v>0.0001912169954066527</v>
+      </c>
+      <c r="K21" t="s">
+        <v>57</v>
+      </c>
+      <c r="L21" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>12</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1.08628</v>
+      </c>
+      <c r="Q21">
+        <v>6.54508</v>
+      </c>
+      <c r="R21" s="2">
+        <v>44040</v>
+      </c>
+      <c r="S21" s="2">
+        <v>45161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22">
+        <v>1.066943238567832</v>
+      </c>
+      <c r="B22">
+        <v>1.066370977662032</v>
+      </c>
+      <c r="C22">
+        <v>1.065890059304828</v>
+      </c>
+      <c r="D22">
+        <v>1.065509235236169</v>
+      </c>
+      <c r="E22">
+        <v>1.065235727571711</v>
+      </c>
+      <c r="F22">
+        <v>1.066943238567832</v>
+      </c>
+      <c r="G22">
+        <v>1.05035</v>
+      </c>
+      <c r="H22">
+        <v>-0.01659323856783179</v>
+      </c>
+      <c r="I22">
+        <v>0.01659323856783179</v>
+      </c>
+      <c r="J22">
+        <v>0.0002753355661689804</v>
+      </c>
+      <c r="K22" t="s">
+        <v>57</v>
+      </c>
+      <c r="L22" t="s">
+        <v>57</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>12</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1.05035</v>
+      </c>
+      <c r="Q22">
+        <v>7.59543</v>
+      </c>
+      <c r="R22" s="2">
+        <v>44075</v>
+      </c>
+      <c r="S22" s="2">
+        <v>45196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23">
+        <v>1.065875402214562</v>
+      </c>
+      <c r="B23">
+        <v>1.066206708418313</v>
+      </c>
+      <c r="C23">
+        <v>1.066536099283072</v>
+      </c>
+      <c r="D23">
+        <v>1.066872370443115</v>
+      </c>
+      <c r="E23">
+        <v>1.067224465211316</v>
+      </c>
+      <c r="F23">
+        <v>1.065875402214562</v>
+      </c>
+      <c r="G23">
+        <v>1.05661</v>
+      </c>
+      <c r="H23">
+        <v>-0.009265402214562402</v>
+      </c>
+      <c r="I23">
+        <v>0.009265402214562402</v>
+      </c>
+      <c r="J23">
+        <v>8.584767819761785E-05</v>
+      </c>
+      <c r="K23" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" t="s">
+        <v>57</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>12</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1.05661</v>
+      </c>
+      <c r="Q23">
+        <v>8.65204</v>
+      </c>
+      <c r="R23" s="2">
+        <v>44110</v>
+      </c>
+      <c r="S23" s="2">
+        <v>45231</v>
       </c>
     </row>
   </sheetData>
@@ -2032,7 +2478,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2051,7 +2497,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2067,7 +2513,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2093,7 +2539,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2189,7 +2635,7 @@
         <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -2197,7 +2643,7 @@
         <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -2205,7 +2651,7 @@
         <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -2269,34 +2715,34 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25">
-        <v>1.059708833694458</v>
+        <v>1.059093475341797</v>
       </c>
       <c r="B25">
-        <v>1.058743834495544</v>
+        <v>1.058691263198853</v>
       </c>
       <c r="C25">
-        <v>1.058047294616699</v>
+        <v>1.058513641357422</v>
       </c>
       <c r="D25">
-        <v>1.057532668113708</v>
+        <v>1.058513998985291</v>
       </c>
       <c r="E25">
-        <v>1.057140350341797</v>
+        <v>1.058646440505981</v>
       </c>
       <c r="F25">
-        <v>1.059708833694458</v>
+        <v>1.059093475341797</v>
       </c>
       <c r="G25">
-        <v>1.05737</v>
+        <v>1.06686</v>
       </c>
       <c r="H25">
-        <v>-0.002338833694458087</v>
+        <v>0.007766524658203044</v>
       </c>
       <c r="I25">
-        <v>0.002338833694458087</v>
+        <v>0.007766524658203044</v>
       </c>
       <c r="J25">
-        <v>5.470143050332463E-06</v>
+        <v>6.031890526647592E-05</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -2308,48 +2754,48 @@
         <v>1</v>
       </c>
       <c r="P25">
-        <v>1.05737</v>
+        <v>1.06686</v>
       </c>
       <c r="Q25">
-        <v>1.05737</v>
+        <v>1.06686</v>
       </c>
       <c r="R25" s="2">
-        <v>43864</v>
+        <v>43865</v>
       </c>
       <c r="S25" s="2">
-        <v>44985</v>
+        <v>44986</v>
       </c>
     </row>
     <row r="26" spans="1:19">
       <c r="A26">
-        <v>1.102564930915833</v>
+        <v>1.090289950370789</v>
       </c>
       <c r="B26">
-        <v>1.102606177330017</v>
+        <v>1.091355323791504</v>
       </c>
       <c r="C26">
-        <v>1.102709412574768</v>
+        <v>1.092228531837463</v>
       </c>
       <c r="D26">
-        <v>1.102855801582336</v>
+        <v>1.092934727668762</v>
       </c>
       <c r="E26">
-        <v>1.103032827377319</v>
+        <v>1.093514442443848</v>
       </c>
       <c r="F26">
-        <v>1.102564930915833</v>
+        <v>1.090289950370789</v>
       </c>
       <c r="G26">
-        <v>1.09597</v>
+        <v>1.09051</v>
       </c>
       <c r="H26">
-        <v>-0.006594930915832631</v>
+        <v>0.0002200496292115162</v>
       </c>
       <c r="I26">
-        <v>0.006594930915832631</v>
+        <v>0.0002200496292115162</v>
       </c>
       <c r="J26">
-        <v>4.349311378460502E-05</v>
+        <v>4.842183931612575E-08</v>
       </c>
       <c r="K26" t="s">
         <v>56</v>
@@ -2367,48 +2813,48 @@
         <v>1</v>
       </c>
       <c r="P26">
-        <v>1.09597</v>
+        <v>1.09051</v>
       </c>
       <c r="Q26">
-        <v>2.15334</v>
+        <v>2.15737</v>
       </c>
       <c r="R26" s="2">
-        <v>43934</v>
+        <v>43900</v>
       </c>
       <c r="S26" s="2">
-        <v>45055</v>
+        <v>45021</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27">
-        <v>1.114355683326721</v>
+        <v>1.100209593772888</v>
       </c>
       <c r="B27">
-        <v>1.118177771568298</v>
+        <v>1.099648952484131</v>
       </c>
       <c r="C27">
-        <v>1.121034145355225</v>
+        <v>1.09923243522644</v>
       </c>
       <c r="D27">
-        <v>1.123148202896118</v>
+        <v>1.09892201423645</v>
       </c>
       <c r="E27">
-        <v>1.124699354171753</v>
+        <v>1.09868323802948</v>
       </c>
       <c r="F27">
-        <v>1.114355683326721</v>
+        <v>1.100209593772888</v>
       </c>
       <c r="G27">
-        <v>1.12275</v>
+        <v>1.09826</v>
       </c>
       <c r="H27">
-        <v>0.008394316673278723</v>
+        <v>-0.00194959377288817</v>
       </c>
       <c r="I27">
-        <v>0.008394316673278723</v>
+        <v>0.00194959377288817</v>
       </c>
       <c r="J27">
-        <v>7.046455241128517E-05</v>
+        <v>3.800915879284328E-06</v>
       </c>
       <c r="K27" t="s">
         <v>56</v>
@@ -2426,48 +2872,48 @@
         <v>1</v>
       </c>
       <c r="P27">
-        <v>1.12275</v>
+        <v>1.09826</v>
       </c>
       <c r="Q27">
-        <v>3.27609</v>
+        <v>3.25563</v>
       </c>
       <c r="R27" s="2">
-        <v>44004</v>
+        <v>43935</v>
       </c>
       <c r="S27" s="2">
-        <v>45125</v>
+        <v>45056</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28">
-        <v>1.06355094909668</v>
+        <v>1.073830008506775</v>
       </c>
       <c r="B28">
-        <v>1.06286609172821</v>
+        <v>1.074546813964844</v>
       </c>
       <c r="C28">
-        <v>1.0623619556427</v>
+        <v>1.075042843818665</v>
       </c>
       <c r="D28">
-        <v>1.061995029449463</v>
+        <v>1.075395822525024</v>
       </c>
       <c r="E28">
-        <v>1.061727523803711</v>
+        <v>1.075646877288818</v>
       </c>
       <c r="F28">
-        <v>1.06355094909668</v>
+        <v>1.073830008506775</v>
       </c>
       <c r="G28">
-        <v>1.05706</v>
+        <v>1.08305</v>
       </c>
       <c r="H28">
-        <v>-0.006490949096679799</v>
+        <v>0.009219991493225166</v>
       </c>
       <c r="I28">
-        <v>0.006490949096679799</v>
+        <v>0.009219991493225166</v>
       </c>
       <c r="J28">
-        <v>4.21324201756883E-05</v>
+        <v>8.500824313514442E-05</v>
       </c>
       <c r="K28" t="s">
         <v>57</v>
@@ -2485,16 +2931,252 @@
         <v>1</v>
       </c>
       <c r="P28">
-        <v>1.05706</v>
+        <v>1.08305</v>
       </c>
       <c r="Q28">
-        <v>4.33315</v>
+        <v>4.33868</v>
       </c>
       <c r="R28" s="2">
-        <v>44074</v>
+        <v>43970</v>
       </c>
       <c r="S28" s="2">
-        <v>45195</v>
+        <v>45091</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29">
+        <v>1.119276285171509</v>
+      </c>
+      <c r="B29">
+        <v>1.121533274650574</v>
+      </c>
+      <c r="C29">
+        <v>1.12311851978302</v>
+      </c>
+      <c r="D29">
+        <v>1.12416136264801</v>
+      </c>
+      <c r="E29">
+        <v>1.124787449836731</v>
+      </c>
+      <c r="F29">
+        <v>1.119276285171509</v>
+      </c>
+      <c r="G29">
+        <v>1.12012</v>
+      </c>
+      <c r="H29">
+        <v>0.0008437148284912155</v>
+      </c>
+      <c r="I29">
+        <v>0.0008437148284912155</v>
+      </c>
+      <c r="J29">
+        <v>7.118547118159612E-07</v>
+      </c>
+      <c r="K29" t="s">
+        <v>56</v>
+      </c>
+      <c r="L29" t="s">
+        <v>56</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>12</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1.12012</v>
+      </c>
+      <c r="Q29">
+        <v>5.4588</v>
+      </c>
+      <c r="R29" s="2">
+        <v>44005</v>
+      </c>
+      <c r="S29" s="2">
+        <v>45126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30">
+        <v>1.086727023124695</v>
+      </c>
+      <c r="B30">
+        <v>1.086249470710754</v>
+      </c>
+      <c r="C30">
+        <v>1.08596658706665</v>
+      </c>
+      <c r="D30">
+        <v>1.085830330848694</v>
+      </c>
+      <c r="E30">
+        <v>1.085796117782593</v>
+      </c>
+      <c r="F30">
+        <v>1.086727023124695</v>
+      </c>
+      <c r="G30">
+        <v>1.08628</v>
+      </c>
+      <c r="H30">
+        <v>-0.0004470231246949119</v>
+      </c>
+      <c r="I30">
+        <v>0.0004470231246949119</v>
+      </c>
+      <c r="J30">
+        <v>1.998296740120027E-07</v>
+      </c>
+      <c r="K30" t="s">
+        <v>57</v>
+      </c>
+      <c r="L30" t="s">
+        <v>57</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>12</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1.08628</v>
+      </c>
+      <c r="Q30">
+        <v>6.54508</v>
+      </c>
+      <c r="R30" s="2">
+        <v>44040</v>
+      </c>
+      <c r="S30" s="2">
+        <v>45161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31">
+        <v>1.061461210250854</v>
+      </c>
+      <c r="B31">
+        <v>1.060432195663452</v>
+      </c>
+      <c r="C31">
+        <v>1.059701561927795</v>
+      </c>
+      <c r="D31">
+        <v>1.0591721534729</v>
+      </c>
+      <c r="E31">
+        <v>1.058782696723938</v>
+      </c>
+      <c r="F31">
+        <v>1.061461210250854</v>
+      </c>
+      <c r="G31">
+        <v>1.05035</v>
+      </c>
+      <c r="H31">
+        <v>-0.0111112102508546</v>
+      </c>
+      <c r="I31">
+        <v>0.0111112102508546</v>
+      </c>
+      <c r="J31">
+        <v>0.0001234589932386963</v>
+      </c>
+      <c r="K31" t="s">
+        <v>57</v>
+      </c>
+      <c r="L31" t="s">
+        <v>57</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>12</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1.05035</v>
+      </c>
+      <c r="Q31">
+        <v>7.59543</v>
+      </c>
+      <c r="R31" s="2">
+        <v>44075</v>
+      </c>
+      <c r="S31" s="2">
+        <v>45196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32">
+        <v>1.0574711561203</v>
+      </c>
+      <c r="B32">
+        <v>1.057303905487061</v>
+      </c>
+      <c r="C32">
+        <v>1.057058930397034</v>
+      </c>
+      <c r="D32">
+        <v>1.056759476661682</v>
+      </c>
+      <c r="E32">
+        <v>1.056421279907227</v>
+      </c>
+      <c r="F32">
+        <v>1.0574711561203</v>
+      </c>
+      <c r="G32">
+        <v>1.05661</v>
+      </c>
+      <c r="H32">
+        <v>-0.0008611561203002438</v>
+      </c>
+      <c r="I32">
+        <v>0.0008611561203002438</v>
+      </c>
+      <c r="J32">
+        <v>7.41589863530568E-07</v>
+      </c>
+      <c r="K32" t="s">
+        <v>56</v>
+      </c>
+      <c r="L32" t="s">
+        <v>57</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>12</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>1.05661</v>
+      </c>
+      <c r="Q32">
+        <v>8.65204</v>
+      </c>
+      <c r="R32" s="2">
+        <v>44110</v>
+      </c>
+      <c r="S32" s="2">
+        <v>45231</v>
       </c>
     </row>
   </sheetData>
@@ -2504,7 +3186,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2512,7 +3194,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -2520,23 +3202,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
         <v>61</v>
@@ -2544,602 +3226,554 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>174</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>176</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>186</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B38" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>188</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B41" t="s">
-        <v>189</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B46" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B49" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B50" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B52" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B53" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B54" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B55" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B56" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B57" t="s">
-        <v>175</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B58" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B59" t="s">
-        <v>179</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B60" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B61" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B62" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B63" t="s">
-        <v>44</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B64" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B65" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B66" t="s">
-        <v>179</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B68" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B69" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B70" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B71" t="s">
-        <v>44</v>
+        <v>206</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B73" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" t="s">
-        <v>160</v>
-      </c>
-      <c r="B74" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
-        <v>161</v>
-      </c>
-      <c r="B75" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
-        <v>162</v>
-      </c>
-      <c r="B76" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
-        <v>163</v>
-      </c>
-      <c r="B77" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
-        <v>164</v>
-      </c>
-      <c r="B78" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
-        <v>165</v>
-      </c>
-      <c r="B79" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>